<commit_message>
First long run OK
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvamiguel/Documents/WORKING/UNIVERSIDAD-OTROS/twitter-sentiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36731923-BB9D-664C-8A5B-7EFEFE576783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7DEA27-DE2C-6B43-885B-F69067A5B4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="33600" windowWidth="60160" windowHeight="33840" xr2:uid="{4C79E745-A53F-C647-9264-492D8FB7534C}"/>
+    <workbookView xWindow="46900" yWindow="37860" windowWidth="28800" windowHeight="17540" xr2:uid="{4C79E745-A53F-C647-9264-492D8FB7534C}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>query</t>
   </si>
@@ -50,6 +50,30 @@
   </si>
   <si>
     <t>#DiaInternacionalAsperger</t>
+  </si>
+  <si>
+    <t>#DíaMundialdelaVisión</t>
+  </si>
+  <si>
+    <t>#DiaMundialAutismo</t>
+  </si>
+  <si>
+    <t>#DiaMundialEnfermedadesRaras</t>
+  </si>
+  <si>
+    <t>#UnFuturoMejor</t>
+  </si>
+  <si>
+    <t>#TDAH</t>
+  </si>
+  <si>
+    <t>#lacausaquenosune</t>
+  </si>
+  <si>
+    <t>#calcetinesdesparejados</t>
+  </si>
+  <si>
+    <t>#DiaNacionalEB</t>
   </si>
 </sst>
 </file>
@@ -85,9 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,15 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0613A17-BDBF-F747-8F7F-C27CA58EC4B0}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -432,14 +460,14 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>44167</v>
+        <v>44166</v>
       </c>
       <c r="C2" s="1">
-        <f>B2+2</f>
-        <v>44169</v>
+        <f>B2+4</f>
+        <v>44170</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -447,14 +475,134 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>43878</v>
+        <v>43877</v>
       </c>
       <c r="C3" s="1">
-        <f>B3+2</f>
-        <v>43880</v>
+        <f t="shared" ref="C3:C11" si="0">B3+4</f>
+        <v>43881</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44129</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>44133</v>
+      </c>
+      <c r="D4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44109</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>44113</v>
+      </c>
+      <c r="D5">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44110</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>44114</v>
+      </c>
+      <c r="D6">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43734</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>43738</v>
+      </c>
+      <c r="D7">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43920</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>43924</v>
+      </c>
+      <c r="D8">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43909</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>43913</v>
+      </c>
+      <c r="D9">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43888</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>43892</v>
+      </c>
+      <c r="D10">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43788</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>43792</v>
+      </c>
+      <c r="D11">
+        <v>40000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>